<commit_message>
Unit Tests for XLSX File Upload
</commit_message>
<xml_diff>
--- a/backend/hct_mis_api/apps/registration_datahub/tests/test_file/Registration Data Import XLS Template.xlsx
+++ b/backend/hct_mis_api/apps/registration_datahub/tests/test_file/Registration Data Import XLS Template.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="257">
   <si>
     <t>This document was exported from Numbers. Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -403,7 +403,7 @@
     <t>Kabul</t>
   </si>
   <si>
-    <t>888-888-8888</t>
+    <t>+44 1632 960852</t>
   </si>
   <si>
     <t>+1-541-754-3010</t>
@@ -442,10 +442,10 @@
     <t>N/A</t>
   </si>
   <si>
-    <t>888-888-8889</t>
-  </si>
-  <si>
-    <t>(541) 754-3010</t>
+    <t>+1-613-555-0182</t>
+  </si>
+  <si>
+    <t>+36 55 979 922</t>
   </si>
   <si>
     <t>Pilar</t>
@@ -475,9 +475,6 @@
     <t>DIVORCED</t>
   </si>
   <si>
-    <t>888-888-8890</t>
-  </si>
-  <si>
     <t>Antony</t>
   </si>
   <si>
@@ -499,9 +496,6 @@
     <t>WIDOW</t>
   </si>
   <si>
-    <t>888-888-8891</t>
-  </si>
-  <si>
     <t>Erasmo</t>
   </si>
   <si>
@@ -526,9 +520,6 @@
     <t>SEPARATED</t>
   </si>
   <si>
-    <t>888-888-8892</t>
-  </si>
-  <si>
     <t>Arvilla</t>
   </si>
   <si>
@@ -544,9 +535,6 @@
     <t>NATIONAL_PASSPORT</t>
   </si>
   <si>
-    <t>888-888-8893</t>
-  </si>
-  <si>
     <t>Junita</t>
   </si>
   <si>
@@ -559,9 +547,6 @@
     <t>24-10-1985</t>
   </si>
   <si>
-    <t>888-888-8894</t>
-  </si>
-  <si>
     <t>Emerald</t>
   </si>
   <si>
@@ -577,9 +562,6 @@
     <t>NOT_AVAILABLE</t>
   </si>
   <si>
-    <t>888-888-8895</t>
-  </si>
-  <si>
     <t>Perla</t>
   </si>
   <si>
@@ -592,9 +574,6 @@
     <t>24-10-1987</t>
   </si>
   <si>
-    <t>888-888-8896</t>
-  </si>
-  <si>
     <t>Russle</t>
   </si>
   <si>
@@ -607,9 +586,6 @@
     <t>24-10-1988</t>
   </si>
   <si>
-    <t>888-888-8897</t>
-  </si>
-  <si>
     <t>Dannie</t>
   </si>
   <si>
@@ -622,9 +598,6 @@
     <t>24-10-1989</t>
   </si>
   <si>
-    <t>888-888-8898</t>
-  </si>
-  <si>
     <t>Breanna</t>
   </si>
   <si>
@@ -637,9 +610,6 @@
     <t>24-10-1990</t>
   </si>
   <si>
-    <t>888-888-8899</t>
-  </si>
-  <si>
     <t>Lisa</t>
   </si>
   <si>
@@ -652,9 +622,6 @@
     <t>24-10-1991</t>
   </si>
   <si>
-    <t>888-888-8900</t>
-  </si>
-  <si>
     <t>Landon</t>
   </si>
   <si>
@@ -667,9 +634,6 @@
     <t>24-10-1992</t>
   </si>
   <si>
-    <t>888-888-8901</t>
-  </si>
-  <si>
     <t>Augusta</t>
   </si>
   <si>
@@ -682,9 +646,6 @@
     <t>24-10-1993</t>
   </si>
   <si>
-    <t>888-888-8902</t>
-  </si>
-  <si>
     <t>Whitley</t>
   </si>
   <si>
@@ -697,9 +658,6 @@
     <t>24-10-1994</t>
   </si>
   <si>
-    <t>888-888-8903</t>
-  </si>
-  <si>
     <t>Cornell</t>
   </si>
   <si>
@@ -712,9 +670,6 @@
     <t>24-10-1995</t>
   </si>
   <si>
-    <t>888-888-8904</t>
-  </si>
-  <si>
     <t>Maryellen</t>
   </si>
   <si>
@@ -727,9 +682,6 @@
     <t>24-10-1996</t>
   </si>
   <si>
-    <t>888-888-8905</t>
-  </si>
-  <si>
     <t>Bonny</t>
   </si>
   <si>
@@ -742,9 +694,6 @@
     <t>24-10-1997</t>
   </si>
   <si>
-    <t>888-888-8906</t>
-  </si>
-  <si>
     <t>Roseanne</t>
   </si>
   <si>
@@ -757,9 +706,6 @@
     <t>24-10-1998</t>
   </si>
   <si>
-    <t>888-888-8907</t>
-  </si>
-  <si>
     <t>Sacha</t>
   </si>
   <si>
@@ -772,9 +718,6 @@
     <t>24-10-1999</t>
   </si>
   <si>
-    <t>888-888-8908</t>
-  </si>
-  <si>
     <t>Bart</t>
   </si>
   <si>
@@ -787,9 +730,6 @@
     <t>24-10-2000</t>
   </si>
   <si>
-    <t>888-888-8909</t>
-  </si>
-  <si>
     <t>Gaylord</t>
   </si>
   <si>
@@ -802,9 +742,6 @@
     <t>24-10-2001</t>
   </si>
   <si>
-    <t>888-888-8910</t>
-  </si>
-  <si>
     <t>Gwyn</t>
   </si>
   <si>
@@ -817,9 +754,6 @@
     <t>24-10-2002</t>
   </si>
   <si>
-    <t>888-888-8911</t>
-  </si>
-  <si>
     <t>Adrian</t>
   </si>
   <si>
@@ -832,9 +766,6 @@
     <t>24-10-2003</t>
   </si>
   <si>
-    <t>888-888-8912</t>
-  </si>
-  <si>
     <t>Marcos</t>
   </si>
   <si>
@@ -847,9 +778,6 @@
     <t>24-10-2004</t>
   </si>
   <si>
-    <t>888-888-8913</t>
-  </si>
-  <si>
     <t>Maurita</t>
   </si>
   <si>
@@ -860,9 +788,6 @@
   </si>
   <si>
     <t>24-10-2005</t>
-  </si>
-  <si>
-    <t>888-888-8914</t>
   </si>
   <si>
     <t>Senaida</t>
@@ -3490,28 +3415,28 @@
         <v>123</v>
       </c>
       <c r="H5" t="s" s="31">
-        <v>148</v>
+        <v>124</v>
       </c>
       <c r="I5" t="s" s="26">
         <v>125</v>
       </c>
       <c r="J5" t="s" s="26">
+        <v>148</v>
+      </c>
+      <c r="K5" t="s" s="26">
         <v>149</v>
-      </c>
-      <c r="K5" t="s" s="26">
-        <v>150</v>
       </c>
       <c r="L5" t="s" s="26">
         <v>128</v>
       </c>
       <c r="M5" t="s" s="26">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="N5" t="s" s="26">
         <v>130</v>
       </c>
       <c r="O5" t="s" s="26">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="P5" s="32">
         <v>38</v>
@@ -3523,13 +3448,13 @@
         <v>43</v>
       </c>
       <c r="S5" t="s" s="26">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="T5" t="s" s="26">
         <v>132</v>
       </c>
       <c r="U5" t="s" s="26">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="V5" t="s" s="26">
         <v>48</v>
@@ -3543,7 +3468,7 @@
         <v>29</v>
       </c>
       <c r="C6" t="s" s="31">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D6" t="s" s="26">
         <v>120</v>
@@ -3558,28 +3483,28 @@
         <v>123</v>
       </c>
       <c r="H6" t="s" s="31">
-        <v>156</v>
+        <v>137</v>
       </c>
       <c r="I6" t="s" s="26">
         <v>138</v>
       </c>
       <c r="J6" t="s" s="26">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="K6" t="s" s="26">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="L6" t="s" s="26">
         <v>128</v>
       </c>
       <c r="M6" t="s" s="26">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="N6" t="s" s="26">
         <v>142</v>
       </c>
       <c r="O6" t="s" s="26">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="P6" s="32">
         <v>37</v>
@@ -3591,16 +3516,16 @@
         <v>29</v>
       </c>
       <c r="S6" t="s" s="26">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="T6" t="s" s="26">
         <v>132</v>
       </c>
       <c r="U6" t="s" s="26">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="V6" t="s" s="26">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="7" ht="24.65" customHeight="1">
@@ -3611,7 +3536,7 @@
         <v>43</v>
       </c>
       <c r="C7" t="s" s="26">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D7" t="s" s="26">
         <v>136</v>
@@ -3626,28 +3551,28 @@
         <v>123</v>
       </c>
       <c r="H7" t="s" s="31">
-        <v>165</v>
+        <v>124</v>
       </c>
       <c r="I7" t="s" s="26">
         <v>125</v>
       </c>
       <c r="J7" t="s" s="26">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="K7" t="s" s="26">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="L7" t="s" s="26">
         <v>128</v>
       </c>
       <c r="M7" t="s" s="26">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="N7" t="s" s="26">
         <v>130</v>
       </c>
       <c r="O7" t="s" s="26">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="P7" s="32">
         <v>36</v>
@@ -3665,7 +3590,7 @@
         <v>132</v>
       </c>
       <c r="U7" t="s" s="26">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="V7" t="s" s="26">
         <v>134</v>
@@ -3694,28 +3619,28 @@
         <v>123</v>
       </c>
       <c r="H8" t="s" s="31">
-        <v>171</v>
+        <v>137</v>
       </c>
       <c r="I8" t="s" s="26">
         <v>138</v>
       </c>
       <c r="J8" t="s" s="26">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="K8" t="s" s="26">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="L8" t="s" s="26">
         <v>128</v>
       </c>
       <c r="M8" t="s" s="26">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="N8" t="s" s="26">
         <v>142</v>
       </c>
       <c r="O8" t="s" s="26">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="P8" s="32">
         <v>35</v>
@@ -3762,28 +3687,28 @@
         <v>123</v>
       </c>
       <c r="H9" t="s" s="31">
-        <v>176</v>
+        <v>124</v>
       </c>
       <c r="I9" t="s" s="26">
         <v>125</v>
       </c>
       <c r="J9" t="s" s="26">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="K9" t="s" s="26">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="L9" t="s" s="26">
         <v>128</v>
       </c>
       <c r="M9" t="s" s="26">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="N9" t="s" s="26">
         <v>130</v>
       </c>
       <c r="O9" t="s" s="26">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="P9" s="32">
         <v>34</v>
@@ -3801,7 +3726,7 @@
         <v>132</v>
       </c>
       <c r="U9" t="s" s="26">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="V9" t="s" s="26">
         <v>48</v>
@@ -3830,28 +3755,28 @@
         <v>123</v>
       </c>
       <c r="H10" t="s" s="31">
-        <v>182</v>
+        <v>137</v>
       </c>
       <c r="I10" t="s" s="26">
         <v>138</v>
       </c>
       <c r="J10" t="s" s="26">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="K10" t="s" s="26">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="L10" t="s" s="26">
         <v>128</v>
       </c>
       <c r="M10" t="s" s="26">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="N10" t="s" s="26">
         <v>142</v>
       </c>
       <c r="O10" t="s" s="26">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="P10" s="32">
         <v>33</v>
@@ -3872,7 +3797,7 @@
         <v>133</v>
       </c>
       <c r="V10" t="s" s="26">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="11" ht="24.65" customHeight="1">
@@ -3883,7 +3808,7 @@
         <v>43</v>
       </c>
       <c r="C11" t="s" s="26">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D11" t="s" s="26">
         <v>136</v>
@@ -3898,28 +3823,28 @@
         <v>123</v>
       </c>
       <c r="H11" t="s" s="31">
-        <v>187</v>
+        <v>124</v>
       </c>
       <c r="I11" t="s" s="26">
         <v>125</v>
       </c>
       <c r="J11" t="s" s="26">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="K11" t="s" s="26">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="L11" t="s" s="26">
         <v>128</v>
       </c>
       <c r="M11" t="s" s="26">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="N11" t="s" s="26">
         <v>130</v>
       </c>
       <c r="O11" t="s" s="26">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="P11" s="32">
         <v>32</v>
@@ -3951,7 +3876,7 @@
         <v>29</v>
       </c>
       <c r="C12" t="s" s="26">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D12" t="s" s="26">
         <v>120</v>
@@ -3966,28 +3891,28 @@
         <v>123</v>
       </c>
       <c r="H12" t="s" s="31">
-        <v>192</v>
+        <v>137</v>
       </c>
       <c r="I12" t="s" s="26">
         <v>138</v>
       </c>
       <c r="J12" t="s" s="26">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="K12" t="s" s="26">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="L12" t="s" s="26">
         <v>128</v>
       </c>
       <c r="M12" t="s" s="26">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="N12" t="s" s="26">
         <v>142</v>
       </c>
       <c r="O12" t="s" s="26">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="P12" s="32">
         <v>31</v>
@@ -3999,13 +3924,13 @@
         <v>29</v>
       </c>
       <c r="S12" t="s" s="26">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="T12" t="s" s="26">
         <v>132</v>
       </c>
       <c r="U12" t="s" s="26">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="V12" t="s" s="26">
         <v>146</v>
@@ -4034,28 +3959,28 @@
         <v>123</v>
       </c>
       <c r="H13" t="s" s="31">
-        <v>197</v>
+        <v>124</v>
       </c>
       <c r="I13" t="s" s="26">
         <v>125</v>
       </c>
       <c r="J13" t="s" s="26">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="K13" t="s" s="26">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="L13" t="s" s="26">
         <v>128</v>
       </c>
       <c r="M13" t="s" s="26">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="N13" t="s" s="26">
         <v>130</v>
       </c>
       <c r="O13" t="s" s="26">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="P13" s="32">
         <v>30</v>
@@ -4067,13 +3992,13 @@
         <v>29</v>
       </c>
       <c r="S13" t="s" s="26">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="T13" t="s" s="26">
         <v>132</v>
       </c>
       <c r="U13" t="s" s="26">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="V13" t="s" s="26">
         <v>48</v>
@@ -4102,28 +4027,28 @@
         <v>123</v>
       </c>
       <c r="H14" t="s" s="31">
-        <v>202</v>
+        <v>137</v>
       </c>
       <c r="I14" t="s" s="26">
         <v>138</v>
       </c>
       <c r="J14" t="s" s="26">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="K14" t="s" s="26">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="L14" t="s" s="26">
         <v>128</v>
       </c>
       <c r="M14" t="s" s="26">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="N14" t="s" s="26">
         <v>142</v>
       </c>
       <c r="O14" t="s" s="26">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="P14" s="32">
         <v>29</v>
@@ -4141,10 +4066,10 @@
         <v>132</v>
       </c>
       <c r="U14" t="s" s="26">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="V14" t="s" s="26">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="15" ht="24.65" customHeight="1">
@@ -4170,28 +4095,28 @@
         <v>123</v>
       </c>
       <c r="H15" t="s" s="31">
-        <v>207</v>
+        <v>124</v>
       </c>
       <c r="I15" t="s" s="26">
         <v>125</v>
       </c>
       <c r="J15" t="s" s="26">
-        <v>208</v>
+        <v>197</v>
       </c>
       <c r="K15" t="s" s="26">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="L15" t="s" s="26">
         <v>128</v>
       </c>
       <c r="M15" t="s" s="26">
-        <v>210</v>
+        <v>199</v>
       </c>
       <c r="N15" t="s" s="26">
         <v>130</v>
       </c>
       <c r="O15" t="s" s="26">
-        <v>211</v>
+        <v>200</v>
       </c>
       <c r="P15" s="32">
         <v>28</v>
@@ -4223,7 +4148,7 @@
         <v>29</v>
       </c>
       <c r="C16" t="s" s="31">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D16" t="s" s="26">
         <v>120</v>
@@ -4238,28 +4163,28 @@
         <v>123</v>
       </c>
       <c r="H16" t="s" s="31">
-        <v>212</v>
+        <v>137</v>
       </c>
       <c r="I16" t="s" s="26">
         <v>138</v>
       </c>
       <c r="J16" t="s" s="26">
-        <v>213</v>
+        <v>201</v>
       </c>
       <c r="K16" t="s" s="26">
-        <v>214</v>
+        <v>202</v>
       </c>
       <c r="L16" t="s" s="26">
         <v>128</v>
       </c>
       <c r="M16" t="s" s="26">
-        <v>215</v>
+        <v>203</v>
       </c>
       <c r="N16" t="s" s="26">
         <v>142</v>
       </c>
       <c r="O16" t="s" s="26">
-        <v>216</v>
+        <v>204</v>
       </c>
       <c r="P16" s="32">
         <v>27</v>
@@ -4277,7 +4202,7 @@
         <v>132</v>
       </c>
       <c r="U16" t="s" s="26">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="V16" t="s" s="26">
         <v>146</v>
@@ -4291,7 +4216,7 @@
         <v>29</v>
       </c>
       <c r="C17" t="s" s="26">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D17" t="s" s="26">
         <v>120</v>
@@ -4306,28 +4231,28 @@
         <v>123</v>
       </c>
       <c r="H17" t="s" s="31">
-        <v>217</v>
+        <v>124</v>
       </c>
       <c r="I17" t="s" s="26">
         <v>125</v>
       </c>
       <c r="J17" t="s" s="26">
-        <v>218</v>
+        <v>205</v>
       </c>
       <c r="K17" t="s" s="26">
-        <v>219</v>
+        <v>206</v>
       </c>
       <c r="L17" t="s" s="26">
         <v>128</v>
       </c>
       <c r="M17" t="s" s="26">
-        <v>220</v>
+        <v>207</v>
       </c>
       <c r="N17" t="s" s="26">
         <v>130</v>
       </c>
       <c r="O17" t="s" s="26">
-        <v>221</v>
+        <v>208</v>
       </c>
       <c r="P17" s="32">
         <v>26</v>
@@ -4374,28 +4299,28 @@
         <v>123</v>
       </c>
       <c r="H18" t="s" s="31">
-        <v>222</v>
+        <v>137</v>
       </c>
       <c r="I18" t="s" s="26">
         <v>138</v>
       </c>
       <c r="J18" t="s" s="26">
-        <v>223</v>
+        <v>209</v>
       </c>
       <c r="K18" t="s" s="26">
-        <v>224</v>
+        <v>210</v>
       </c>
       <c r="L18" t="s" s="26">
         <v>128</v>
       </c>
       <c r="M18" t="s" s="26">
-        <v>225</v>
+        <v>211</v>
       </c>
       <c r="N18" t="s" s="26">
         <v>142</v>
       </c>
       <c r="O18" t="s" s="26">
-        <v>226</v>
+        <v>212</v>
       </c>
       <c r="P18" s="32">
         <v>25</v>
@@ -4407,7 +4332,7 @@
         <v>29</v>
       </c>
       <c r="S18" t="s" s="26">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="T18" t="s" s="26">
         <v>132</v>
@@ -4416,7 +4341,7 @@
         <v>145</v>
       </c>
       <c r="V18" t="s" s="26">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="19" ht="24.65" customHeight="1">
@@ -4442,28 +4367,28 @@
         <v>123</v>
       </c>
       <c r="H19" t="s" s="31">
-        <v>227</v>
+        <v>124</v>
       </c>
       <c r="I19" t="s" s="26">
         <v>125</v>
       </c>
       <c r="J19" t="s" s="26">
-        <v>228</v>
+        <v>213</v>
       </c>
       <c r="K19" t="s" s="26">
-        <v>229</v>
+        <v>214</v>
       </c>
       <c r="L19" t="s" s="26">
         <v>128</v>
       </c>
       <c r="M19" t="s" s="26">
-        <v>230</v>
+        <v>215</v>
       </c>
       <c r="N19" t="s" s="26">
         <v>130</v>
       </c>
       <c r="O19" t="s" s="26">
-        <v>231</v>
+        <v>216</v>
       </c>
       <c r="P19" s="32">
         <v>24</v>
@@ -4475,13 +4400,13 @@
         <v>29</v>
       </c>
       <c r="S19" t="s" s="26">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="T19" t="s" s="26">
         <v>132</v>
       </c>
       <c r="U19" t="s" s="26">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="V19" t="s" s="26">
         <v>134</v>
@@ -4510,28 +4435,28 @@
         <v>123</v>
       </c>
       <c r="H20" t="s" s="31">
-        <v>232</v>
+        <v>137</v>
       </c>
       <c r="I20" t="s" s="26">
         <v>138</v>
       </c>
       <c r="J20" t="s" s="26">
-        <v>233</v>
+        <v>217</v>
       </c>
       <c r="K20" t="s" s="26">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="L20" t="s" s="26">
         <v>128</v>
       </c>
       <c r="M20" t="s" s="26">
-        <v>235</v>
+        <v>219</v>
       </c>
       <c r="N20" t="s" s="26">
         <v>142</v>
       </c>
       <c r="O20" t="s" s="26">
-        <v>236</v>
+        <v>220</v>
       </c>
       <c r="P20" s="32">
         <v>23</v>
@@ -4549,7 +4474,7 @@
         <v>132</v>
       </c>
       <c r="U20" t="s" s="26">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="V20" t="s" s="26">
         <v>146</v>
@@ -4563,7 +4488,7 @@
         <v>29</v>
       </c>
       <c r="C21" t="s" s="31">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D21" t="s" s="26">
         <v>120</v>
@@ -4578,28 +4503,28 @@
         <v>123</v>
       </c>
       <c r="H21" t="s" s="31">
-        <v>237</v>
+        <v>124</v>
       </c>
       <c r="I21" t="s" s="26">
         <v>125</v>
       </c>
       <c r="J21" t="s" s="26">
-        <v>238</v>
+        <v>221</v>
       </c>
       <c r="K21" t="s" s="26">
-        <v>239</v>
+        <v>222</v>
       </c>
       <c r="L21" t="s" s="26">
         <v>128</v>
       </c>
       <c r="M21" t="s" s="26">
-        <v>240</v>
+        <v>223</v>
       </c>
       <c r="N21" t="s" s="26">
         <v>130</v>
       </c>
       <c r="O21" t="s" s="26">
-        <v>241</v>
+        <v>224</v>
       </c>
       <c r="P21" s="32">
         <v>22</v>
@@ -4611,13 +4536,13 @@
         <v>29</v>
       </c>
       <c r="S21" t="s" s="26">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="T21" t="s" s="26">
         <v>132</v>
       </c>
       <c r="U21" t="s" s="26">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="V21" t="s" s="26">
         <v>48</v>
@@ -4631,7 +4556,7 @@
         <v>29</v>
       </c>
       <c r="C22" t="s" s="26">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D22" t="s" s="26">
         <v>120</v>
@@ -4646,28 +4571,28 @@
         <v>123</v>
       </c>
       <c r="H22" t="s" s="31">
-        <v>242</v>
+        <v>137</v>
       </c>
       <c r="I22" t="s" s="26">
         <v>138</v>
       </c>
       <c r="J22" t="s" s="26">
-        <v>243</v>
+        <v>225</v>
       </c>
       <c r="K22" t="s" s="26">
-        <v>244</v>
+        <v>226</v>
       </c>
       <c r="L22" t="s" s="26">
         <v>128</v>
       </c>
       <c r="M22" t="s" s="26">
-        <v>245</v>
+        <v>227</v>
       </c>
       <c r="N22" t="s" s="26">
         <v>142</v>
       </c>
       <c r="O22" t="s" s="26">
-        <v>246</v>
+        <v>228</v>
       </c>
       <c r="P22" s="32">
         <v>21</v>
@@ -4679,7 +4604,7 @@
         <v>29</v>
       </c>
       <c r="S22" t="s" s="26">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="T22" t="s" s="26">
         <v>132</v>
@@ -4688,7 +4613,7 @@
         <v>48</v>
       </c>
       <c r="V22" t="s" s="26">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="23" ht="24.65" customHeight="1">
@@ -4714,28 +4639,28 @@
         <v>123</v>
       </c>
       <c r="H23" t="s" s="31">
-        <v>247</v>
+        <v>124</v>
       </c>
       <c r="I23" t="s" s="26">
         <v>125</v>
       </c>
       <c r="J23" t="s" s="26">
-        <v>248</v>
+        <v>229</v>
       </c>
       <c r="K23" t="s" s="26">
-        <v>249</v>
+        <v>230</v>
       </c>
       <c r="L23" t="s" s="26">
         <v>128</v>
       </c>
       <c r="M23" t="s" s="26">
-        <v>250</v>
+        <v>231</v>
       </c>
       <c r="N23" t="s" s="26">
         <v>130</v>
       </c>
       <c r="O23" t="s" s="26">
-        <v>251</v>
+        <v>232</v>
       </c>
       <c r="P23" s="32">
         <v>20</v>
@@ -4753,7 +4678,7 @@
         <v>132</v>
       </c>
       <c r="U23" t="s" s="26">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="V23" t="s" s="26">
         <v>134</v>
@@ -4782,28 +4707,28 @@
         <v>123</v>
       </c>
       <c r="H24" t="s" s="31">
-        <v>252</v>
+        <v>137</v>
       </c>
       <c r="I24" t="s" s="26">
         <v>138</v>
       </c>
       <c r="J24" t="s" s="26">
-        <v>253</v>
+        <v>233</v>
       </c>
       <c r="K24" t="s" s="26">
-        <v>254</v>
+        <v>234</v>
       </c>
       <c r="L24" t="s" s="26">
         <v>128</v>
       </c>
       <c r="M24" t="s" s="26">
-        <v>255</v>
+        <v>235</v>
       </c>
       <c r="N24" t="s" s="26">
         <v>142</v>
       </c>
       <c r="O24" t="s" s="26">
-        <v>256</v>
+        <v>236</v>
       </c>
       <c r="P24" s="32">
         <v>19</v>
@@ -4850,28 +4775,28 @@
         <v>123</v>
       </c>
       <c r="H25" t="s" s="31">
-        <v>257</v>
+        <v>124</v>
       </c>
       <c r="I25" t="s" s="26">
         <v>125</v>
       </c>
       <c r="J25" t="s" s="26">
-        <v>258</v>
+        <v>237</v>
       </c>
       <c r="K25" t="s" s="26">
-        <v>259</v>
+        <v>238</v>
       </c>
       <c r="L25" t="s" s="26">
         <v>128</v>
       </c>
       <c r="M25" t="s" s="26">
-        <v>260</v>
+        <v>239</v>
       </c>
       <c r="N25" t="s" s="26">
         <v>130</v>
       </c>
       <c r="O25" t="s" s="26">
-        <v>261</v>
+        <v>240</v>
       </c>
       <c r="P25" s="32">
         <v>18</v>
@@ -4903,7 +4828,7 @@
         <v>29</v>
       </c>
       <c r="C26" t="s" s="31">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D26" t="s" s="26">
         <v>120</v>
@@ -4918,28 +4843,28 @@
         <v>123</v>
       </c>
       <c r="H26" t="s" s="31">
-        <v>262</v>
+        <v>137</v>
       </c>
       <c r="I26" t="s" s="26">
         <v>138</v>
       </c>
       <c r="J26" t="s" s="26">
-        <v>263</v>
+        <v>241</v>
       </c>
       <c r="K26" t="s" s="26">
-        <v>264</v>
+        <v>242</v>
       </c>
       <c r="L26" t="s" s="26">
         <v>128</v>
       </c>
       <c r="M26" t="s" s="26">
-        <v>265</v>
+        <v>243</v>
       </c>
       <c r="N26" t="s" s="26">
         <v>142</v>
       </c>
       <c r="O26" t="s" s="26">
-        <v>266</v>
+        <v>244</v>
       </c>
       <c r="P26" s="32">
         <v>17</v>
@@ -4957,10 +4882,10 @@
         <v>132</v>
       </c>
       <c r="U26" t="s" s="26">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="V26" t="s" s="26">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="27" ht="24.65" customHeight="1">
@@ -4971,7 +4896,7 @@
         <v>29</v>
       </c>
       <c r="C27" t="s" s="26">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D27" t="s" s="26">
         <v>120</v>
@@ -4986,28 +4911,28 @@
         <v>123</v>
       </c>
       <c r="H27" t="s" s="31">
-        <v>267</v>
+        <v>124</v>
       </c>
       <c r="I27" t="s" s="26">
         <v>125</v>
       </c>
       <c r="J27" t="s" s="26">
-        <v>268</v>
+        <v>245</v>
       </c>
       <c r="K27" t="s" s="26">
-        <v>269</v>
+        <v>246</v>
       </c>
       <c r="L27" t="s" s="26">
         <v>128</v>
       </c>
       <c r="M27" t="s" s="26">
-        <v>270</v>
+        <v>247</v>
       </c>
       <c r="N27" t="s" s="26">
         <v>130</v>
       </c>
       <c r="O27" t="s" s="26">
-        <v>271</v>
+        <v>248</v>
       </c>
       <c r="P27" s="32">
         <v>16</v>
@@ -5019,13 +4944,13 @@
         <v>29</v>
       </c>
       <c r="S27" t="s" s="26">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="T27" t="s" s="26">
         <v>132</v>
       </c>
       <c r="U27" t="s" s="26">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="V27" t="s" s="26">
         <v>134</v>
@@ -5054,28 +4979,28 @@
         <v>123</v>
       </c>
       <c r="H28" t="s" s="31">
-        <v>272</v>
+        <v>137</v>
       </c>
       <c r="I28" t="s" s="26">
         <v>138</v>
       </c>
       <c r="J28" t="s" s="26">
-        <v>273</v>
+        <v>249</v>
       </c>
       <c r="K28" t="s" s="26">
-        <v>274</v>
+        <v>250</v>
       </c>
       <c r="L28" t="s" s="26">
         <v>128</v>
       </c>
       <c r="M28" t="s" s="26">
-        <v>275</v>
+        <v>251</v>
       </c>
       <c r="N28" t="s" s="26">
         <v>142</v>
       </c>
       <c r="O28" t="s" s="26">
-        <v>276</v>
+        <v>252</v>
       </c>
       <c r="P28" s="32">
         <v>15</v>
@@ -5093,7 +5018,7 @@
         <v>132</v>
       </c>
       <c r="U28" t="s" s="26">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="V28" t="s" s="26">
         <v>146</v>
@@ -5122,28 +5047,28 @@
         <v>123</v>
       </c>
       <c r="H29" t="s" s="31">
-        <v>277</v>
+        <v>124</v>
       </c>
       <c r="I29" t="s" s="26">
         <v>125</v>
       </c>
       <c r="J29" t="s" s="26">
-        <v>278</v>
+        <v>253</v>
       </c>
       <c r="K29" t="s" s="26">
-        <v>279</v>
+        <v>254</v>
       </c>
       <c r="L29" t="s" s="26">
         <v>128</v>
       </c>
       <c r="M29" t="s" s="26">
-        <v>280</v>
+        <v>255</v>
       </c>
       <c r="N29" t="s" s="26">
         <v>130</v>
       </c>
       <c r="O29" t="s" s="26">
-        <v>281</v>
+        <v>256</v>
       </c>
       <c r="P29" s="32">
         <v>14</v>

</xml_diff>

<commit_message>
Unit Tests for XLSX File Upload (#140)
</commit_message>
<xml_diff>
--- a/backend/hct_mis_api/apps/registration_datahub/tests/test_file/Registration Data Import XLS Template.xlsx
+++ b/backend/hct_mis_api/apps/registration_datahub/tests/test_file/Registration Data Import XLS Template.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="257">
   <si>
     <t>This document was exported from Numbers. Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -403,7 +403,7 @@
     <t>Kabul</t>
   </si>
   <si>
-    <t>888-888-8888</t>
+    <t>+44 1632 960852</t>
   </si>
   <si>
     <t>+1-541-754-3010</t>
@@ -442,10 +442,10 @@
     <t>N/A</t>
   </si>
   <si>
-    <t>888-888-8889</t>
-  </si>
-  <si>
-    <t>(541) 754-3010</t>
+    <t>+1-613-555-0182</t>
+  </si>
+  <si>
+    <t>+36 55 979 922</t>
   </si>
   <si>
     <t>Pilar</t>
@@ -475,9 +475,6 @@
     <t>DIVORCED</t>
   </si>
   <si>
-    <t>888-888-8890</t>
-  </si>
-  <si>
     <t>Antony</t>
   </si>
   <si>
@@ -499,9 +496,6 @@
     <t>WIDOW</t>
   </si>
   <si>
-    <t>888-888-8891</t>
-  </si>
-  <si>
     <t>Erasmo</t>
   </si>
   <si>
@@ -526,9 +520,6 @@
     <t>SEPARATED</t>
   </si>
   <si>
-    <t>888-888-8892</t>
-  </si>
-  <si>
     <t>Arvilla</t>
   </si>
   <si>
@@ -544,9 +535,6 @@
     <t>NATIONAL_PASSPORT</t>
   </si>
   <si>
-    <t>888-888-8893</t>
-  </si>
-  <si>
     <t>Junita</t>
   </si>
   <si>
@@ -559,9 +547,6 @@
     <t>24-10-1985</t>
   </si>
   <si>
-    <t>888-888-8894</t>
-  </si>
-  <si>
     <t>Emerald</t>
   </si>
   <si>
@@ -577,9 +562,6 @@
     <t>NOT_AVAILABLE</t>
   </si>
   <si>
-    <t>888-888-8895</t>
-  </si>
-  <si>
     <t>Perla</t>
   </si>
   <si>
@@ -592,9 +574,6 @@
     <t>24-10-1987</t>
   </si>
   <si>
-    <t>888-888-8896</t>
-  </si>
-  <si>
     <t>Russle</t>
   </si>
   <si>
@@ -607,9 +586,6 @@
     <t>24-10-1988</t>
   </si>
   <si>
-    <t>888-888-8897</t>
-  </si>
-  <si>
     <t>Dannie</t>
   </si>
   <si>
@@ -622,9 +598,6 @@
     <t>24-10-1989</t>
   </si>
   <si>
-    <t>888-888-8898</t>
-  </si>
-  <si>
     <t>Breanna</t>
   </si>
   <si>
@@ -637,9 +610,6 @@
     <t>24-10-1990</t>
   </si>
   <si>
-    <t>888-888-8899</t>
-  </si>
-  <si>
     <t>Lisa</t>
   </si>
   <si>
@@ -652,9 +622,6 @@
     <t>24-10-1991</t>
   </si>
   <si>
-    <t>888-888-8900</t>
-  </si>
-  <si>
     <t>Landon</t>
   </si>
   <si>
@@ -667,9 +634,6 @@
     <t>24-10-1992</t>
   </si>
   <si>
-    <t>888-888-8901</t>
-  </si>
-  <si>
     <t>Augusta</t>
   </si>
   <si>
@@ -682,9 +646,6 @@
     <t>24-10-1993</t>
   </si>
   <si>
-    <t>888-888-8902</t>
-  </si>
-  <si>
     <t>Whitley</t>
   </si>
   <si>
@@ -697,9 +658,6 @@
     <t>24-10-1994</t>
   </si>
   <si>
-    <t>888-888-8903</t>
-  </si>
-  <si>
     <t>Cornell</t>
   </si>
   <si>
@@ -712,9 +670,6 @@
     <t>24-10-1995</t>
   </si>
   <si>
-    <t>888-888-8904</t>
-  </si>
-  <si>
     <t>Maryellen</t>
   </si>
   <si>
@@ -727,9 +682,6 @@
     <t>24-10-1996</t>
   </si>
   <si>
-    <t>888-888-8905</t>
-  </si>
-  <si>
     <t>Bonny</t>
   </si>
   <si>
@@ -742,9 +694,6 @@
     <t>24-10-1997</t>
   </si>
   <si>
-    <t>888-888-8906</t>
-  </si>
-  <si>
     <t>Roseanne</t>
   </si>
   <si>
@@ -757,9 +706,6 @@
     <t>24-10-1998</t>
   </si>
   <si>
-    <t>888-888-8907</t>
-  </si>
-  <si>
     <t>Sacha</t>
   </si>
   <si>
@@ -772,9 +718,6 @@
     <t>24-10-1999</t>
   </si>
   <si>
-    <t>888-888-8908</t>
-  </si>
-  <si>
     <t>Bart</t>
   </si>
   <si>
@@ -787,9 +730,6 @@
     <t>24-10-2000</t>
   </si>
   <si>
-    <t>888-888-8909</t>
-  </si>
-  <si>
     <t>Gaylord</t>
   </si>
   <si>
@@ -802,9 +742,6 @@
     <t>24-10-2001</t>
   </si>
   <si>
-    <t>888-888-8910</t>
-  </si>
-  <si>
     <t>Gwyn</t>
   </si>
   <si>
@@ -817,9 +754,6 @@
     <t>24-10-2002</t>
   </si>
   <si>
-    <t>888-888-8911</t>
-  </si>
-  <si>
     <t>Adrian</t>
   </si>
   <si>
@@ -832,9 +766,6 @@
     <t>24-10-2003</t>
   </si>
   <si>
-    <t>888-888-8912</t>
-  </si>
-  <si>
     <t>Marcos</t>
   </si>
   <si>
@@ -847,9 +778,6 @@
     <t>24-10-2004</t>
   </si>
   <si>
-    <t>888-888-8913</t>
-  </si>
-  <si>
     <t>Maurita</t>
   </si>
   <si>
@@ -860,9 +788,6 @@
   </si>
   <si>
     <t>24-10-2005</t>
-  </si>
-  <si>
-    <t>888-888-8914</t>
   </si>
   <si>
     <t>Senaida</t>
@@ -3490,28 +3415,28 @@
         <v>123</v>
       </c>
       <c r="H5" t="s" s="31">
-        <v>148</v>
+        <v>124</v>
       </c>
       <c r="I5" t="s" s="26">
         <v>125</v>
       </c>
       <c r="J5" t="s" s="26">
+        <v>148</v>
+      </c>
+      <c r="K5" t="s" s="26">
         <v>149</v>
-      </c>
-      <c r="K5" t="s" s="26">
-        <v>150</v>
       </c>
       <c r="L5" t="s" s="26">
         <v>128</v>
       </c>
       <c r="M5" t="s" s="26">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="N5" t="s" s="26">
         <v>130</v>
       </c>
       <c r="O5" t="s" s="26">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="P5" s="32">
         <v>38</v>
@@ -3523,13 +3448,13 @@
         <v>43</v>
       </c>
       <c r="S5" t="s" s="26">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="T5" t="s" s="26">
         <v>132</v>
       </c>
       <c r="U5" t="s" s="26">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="V5" t="s" s="26">
         <v>48</v>
@@ -3543,7 +3468,7 @@
         <v>29</v>
       </c>
       <c r="C6" t="s" s="31">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D6" t="s" s="26">
         <v>120</v>
@@ -3558,28 +3483,28 @@
         <v>123</v>
       </c>
       <c r="H6" t="s" s="31">
-        <v>156</v>
+        <v>137</v>
       </c>
       <c r="I6" t="s" s="26">
         <v>138</v>
       </c>
       <c r="J6" t="s" s="26">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="K6" t="s" s="26">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="L6" t="s" s="26">
         <v>128</v>
       </c>
       <c r="M6" t="s" s="26">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="N6" t="s" s="26">
         <v>142</v>
       </c>
       <c r="O6" t="s" s="26">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="P6" s="32">
         <v>37</v>
@@ -3591,16 +3516,16 @@
         <v>29</v>
       </c>
       <c r="S6" t="s" s="26">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="T6" t="s" s="26">
         <v>132</v>
       </c>
       <c r="U6" t="s" s="26">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="V6" t="s" s="26">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="7" ht="24.65" customHeight="1">
@@ -3611,7 +3536,7 @@
         <v>43</v>
       </c>
       <c r="C7" t="s" s="26">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D7" t="s" s="26">
         <v>136</v>
@@ -3626,28 +3551,28 @@
         <v>123</v>
       </c>
       <c r="H7" t="s" s="31">
-        <v>165</v>
+        <v>124</v>
       </c>
       <c r="I7" t="s" s="26">
         <v>125</v>
       </c>
       <c r="J7" t="s" s="26">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="K7" t="s" s="26">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="L7" t="s" s="26">
         <v>128</v>
       </c>
       <c r="M7" t="s" s="26">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="N7" t="s" s="26">
         <v>130</v>
       </c>
       <c r="O7" t="s" s="26">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="P7" s="32">
         <v>36</v>
@@ -3665,7 +3590,7 @@
         <v>132</v>
       </c>
       <c r="U7" t="s" s="26">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="V7" t="s" s="26">
         <v>134</v>
@@ -3694,28 +3619,28 @@
         <v>123</v>
       </c>
       <c r="H8" t="s" s="31">
-        <v>171</v>
+        <v>137</v>
       </c>
       <c r="I8" t="s" s="26">
         <v>138</v>
       </c>
       <c r="J8" t="s" s="26">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="K8" t="s" s="26">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="L8" t="s" s="26">
         <v>128</v>
       </c>
       <c r="M8" t="s" s="26">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="N8" t="s" s="26">
         <v>142</v>
       </c>
       <c r="O8" t="s" s="26">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="P8" s="32">
         <v>35</v>
@@ -3762,28 +3687,28 @@
         <v>123</v>
       </c>
       <c r="H9" t="s" s="31">
-        <v>176</v>
+        <v>124</v>
       </c>
       <c r="I9" t="s" s="26">
         <v>125</v>
       </c>
       <c r="J9" t="s" s="26">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="K9" t="s" s="26">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="L9" t="s" s="26">
         <v>128</v>
       </c>
       <c r="M9" t="s" s="26">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="N9" t="s" s="26">
         <v>130</v>
       </c>
       <c r="O9" t="s" s="26">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="P9" s="32">
         <v>34</v>
@@ -3801,7 +3726,7 @@
         <v>132</v>
       </c>
       <c r="U9" t="s" s="26">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="V9" t="s" s="26">
         <v>48</v>
@@ -3830,28 +3755,28 @@
         <v>123</v>
       </c>
       <c r="H10" t="s" s="31">
-        <v>182</v>
+        <v>137</v>
       </c>
       <c r="I10" t="s" s="26">
         <v>138</v>
       </c>
       <c r="J10" t="s" s="26">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="K10" t="s" s="26">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="L10" t="s" s="26">
         <v>128</v>
       </c>
       <c r="M10" t="s" s="26">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="N10" t="s" s="26">
         <v>142</v>
       </c>
       <c r="O10" t="s" s="26">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="P10" s="32">
         <v>33</v>
@@ -3872,7 +3797,7 @@
         <v>133</v>
       </c>
       <c r="V10" t="s" s="26">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="11" ht="24.65" customHeight="1">
@@ -3883,7 +3808,7 @@
         <v>43</v>
       </c>
       <c r="C11" t="s" s="26">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D11" t="s" s="26">
         <v>136</v>
@@ -3898,28 +3823,28 @@
         <v>123</v>
       </c>
       <c r="H11" t="s" s="31">
-        <v>187</v>
+        <v>124</v>
       </c>
       <c r="I11" t="s" s="26">
         <v>125</v>
       </c>
       <c r="J11" t="s" s="26">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="K11" t="s" s="26">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="L11" t="s" s="26">
         <v>128</v>
       </c>
       <c r="M11" t="s" s="26">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="N11" t="s" s="26">
         <v>130</v>
       </c>
       <c r="O11" t="s" s="26">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="P11" s="32">
         <v>32</v>
@@ -3951,7 +3876,7 @@
         <v>29</v>
       </c>
       <c r="C12" t="s" s="26">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D12" t="s" s="26">
         <v>120</v>
@@ -3966,28 +3891,28 @@
         <v>123</v>
       </c>
       <c r="H12" t="s" s="31">
-        <v>192</v>
+        <v>137</v>
       </c>
       <c r="I12" t="s" s="26">
         <v>138</v>
       </c>
       <c r="J12" t="s" s="26">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="K12" t="s" s="26">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="L12" t="s" s="26">
         <v>128</v>
       </c>
       <c r="M12" t="s" s="26">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="N12" t="s" s="26">
         <v>142</v>
       </c>
       <c r="O12" t="s" s="26">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="P12" s="32">
         <v>31</v>
@@ -3999,13 +3924,13 @@
         <v>29</v>
       </c>
       <c r="S12" t="s" s="26">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="T12" t="s" s="26">
         <v>132</v>
       </c>
       <c r="U12" t="s" s="26">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="V12" t="s" s="26">
         <v>146</v>
@@ -4034,28 +3959,28 @@
         <v>123</v>
       </c>
       <c r="H13" t="s" s="31">
-        <v>197</v>
+        <v>124</v>
       </c>
       <c r="I13" t="s" s="26">
         <v>125</v>
       </c>
       <c r="J13" t="s" s="26">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="K13" t="s" s="26">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="L13" t="s" s="26">
         <v>128</v>
       </c>
       <c r="M13" t="s" s="26">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="N13" t="s" s="26">
         <v>130</v>
       </c>
       <c r="O13" t="s" s="26">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="P13" s="32">
         <v>30</v>
@@ -4067,13 +3992,13 @@
         <v>29</v>
       </c>
       <c r="S13" t="s" s="26">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="T13" t="s" s="26">
         <v>132</v>
       </c>
       <c r="U13" t="s" s="26">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="V13" t="s" s="26">
         <v>48</v>
@@ -4102,28 +4027,28 @@
         <v>123</v>
       </c>
       <c r="H14" t="s" s="31">
-        <v>202</v>
+        <v>137</v>
       </c>
       <c r="I14" t="s" s="26">
         <v>138</v>
       </c>
       <c r="J14" t="s" s="26">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="K14" t="s" s="26">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="L14" t="s" s="26">
         <v>128</v>
       </c>
       <c r="M14" t="s" s="26">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="N14" t="s" s="26">
         <v>142</v>
       </c>
       <c r="O14" t="s" s="26">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="P14" s="32">
         <v>29</v>
@@ -4141,10 +4066,10 @@
         <v>132</v>
       </c>
       <c r="U14" t="s" s="26">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="V14" t="s" s="26">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="15" ht="24.65" customHeight="1">
@@ -4170,28 +4095,28 @@
         <v>123</v>
       </c>
       <c r="H15" t="s" s="31">
-        <v>207</v>
+        <v>124</v>
       </c>
       <c r="I15" t="s" s="26">
         <v>125</v>
       </c>
       <c r="J15" t="s" s="26">
-        <v>208</v>
+        <v>197</v>
       </c>
       <c r="K15" t="s" s="26">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="L15" t="s" s="26">
         <v>128</v>
       </c>
       <c r="M15" t="s" s="26">
-        <v>210</v>
+        <v>199</v>
       </c>
       <c r="N15" t="s" s="26">
         <v>130</v>
       </c>
       <c r="O15" t="s" s="26">
-        <v>211</v>
+        <v>200</v>
       </c>
       <c r="P15" s="32">
         <v>28</v>
@@ -4223,7 +4148,7 @@
         <v>29</v>
       </c>
       <c r="C16" t="s" s="31">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D16" t="s" s="26">
         <v>120</v>
@@ -4238,28 +4163,28 @@
         <v>123</v>
       </c>
       <c r="H16" t="s" s="31">
-        <v>212</v>
+        <v>137</v>
       </c>
       <c r="I16" t="s" s="26">
         <v>138</v>
       </c>
       <c r="J16" t="s" s="26">
-        <v>213</v>
+        <v>201</v>
       </c>
       <c r="K16" t="s" s="26">
-        <v>214</v>
+        <v>202</v>
       </c>
       <c r="L16" t="s" s="26">
         <v>128</v>
       </c>
       <c r="M16" t="s" s="26">
-        <v>215</v>
+        <v>203</v>
       </c>
       <c r="N16" t="s" s="26">
         <v>142</v>
       </c>
       <c r="O16" t="s" s="26">
-        <v>216</v>
+        <v>204</v>
       </c>
       <c r="P16" s="32">
         <v>27</v>
@@ -4277,7 +4202,7 @@
         <v>132</v>
       </c>
       <c r="U16" t="s" s="26">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="V16" t="s" s="26">
         <v>146</v>
@@ -4291,7 +4216,7 @@
         <v>29</v>
       </c>
       <c r="C17" t="s" s="26">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D17" t="s" s="26">
         <v>120</v>
@@ -4306,28 +4231,28 @@
         <v>123</v>
       </c>
       <c r="H17" t="s" s="31">
-        <v>217</v>
+        <v>124</v>
       </c>
       <c r="I17" t="s" s="26">
         <v>125</v>
       </c>
       <c r="J17" t="s" s="26">
-        <v>218</v>
+        <v>205</v>
       </c>
       <c r="K17" t="s" s="26">
-        <v>219</v>
+        <v>206</v>
       </c>
       <c r="L17" t="s" s="26">
         <v>128</v>
       </c>
       <c r="M17" t="s" s="26">
-        <v>220</v>
+        <v>207</v>
       </c>
       <c r="N17" t="s" s="26">
         <v>130</v>
       </c>
       <c r="O17" t="s" s="26">
-        <v>221</v>
+        <v>208</v>
       </c>
       <c r="P17" s="32">
         <v>26</v>
@@ -4374,28 +4299,28 @@
         <v>123</v>
       </c>
       <c r="H18" t="s" s="31">
-        <v>222</v>
+        <v>137</v>
       </c>
       <c r="I18" t="s" s="26">
         <v>138</v>
       </c>
       <c r="J18" t="s" s="26">
-        <v>223</v>
+        <v>209</v>
       </c>
       <c r="K18" t="s" s="26">
-        <v>224</v>
+        <v>210</v>
       </c>
       <c r="L18" t="s" s="26">
         <v>128</v>
       </c>
       <c r="M18" t="s" s="26">
-        <v>225</v>
+        <v>211</v>
       </c>
       <c r="N18" t="s" s="26">
         <v>142</v>
       </c>
       <c r="O18" t="s" s="26">
-        <v>226</v>
+        <v>212</v>
       </c>
       <c r="P18" s="32">
         <v>25</v>
@@ -4407,7 +4332,7 @@
         <v>29</v>
       </c>
       <c r="S18" t="s" s="26">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="T18" t="s" s="26">
         <v>132</v>
@@ -4416,7 +4341,7 @@
         <v>145</v>
       </c>
       <c r="V18" t="s" s="26">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="19" ht="24.65" customHeight="1">
@@ -4442,28 +4367,28 @@
         <v>123</v>
       </c>
       <c r="H19" t="s" s="31">
-        <v>227</v>
+        <v>124</v>
       </c>
       <c r="I19" t="s" s="26">
         <v>125</v>
       </c>
       <c r="J19" t="s" s="26">
-        <v>228</v>
+        <v>213</v>
       </c>
       <c r="K19" t="s" s="26">
-        <v>229</v>
+        <v>214</v>
       </c>
       <c r="L19" t="s" s="26">
         <v>128</v>
       </c>
       <c r="M19" t="s" s="26">
-        <v>230</v>
+        <v>215</v>
       </c>
       <c r="N19" t="s" s="26">
         <v>130</v>
       </c>
       <c r="O19" t="s" s="26">
-        <v>231</v>
+        <v>216</v>
       </c>
       <c r="P19" s="32">
         <v>24</v>
@@ -4475,13 +4400,13 @@
         <v>29</v>
       </c>
       <c r="S19" t="s" s="26">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="T19" t="s" s="26">
         <v>132</v>
       </c>
       <c r="U19" t="s" s="26">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="V19" t="s" s="26">
         <v>134</v>
@@ -4510,28 +4435,28 @@
         <v>123</v>
       </c>
       <c r="H20" t="s" s="31">
-        <v>232</v>
+        <v>137</v>
       </c>
       <c r="I20" t="s" s="26">
         <v>138</v>
       </c>
       <c r="J20" t="s" s="26">
-        <v>233</v>
+        <v>217</v>
       </c>
       <c r="K20" t="s" s="26">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="L20" t="s" s="26">
         <v>128</v>
       </c>
       <c r="M20" t="s" s="26">
-        <v>235</v>
+        <v>219</v>
       </c>
       <c r="N20" t="s" s="26">
         <v>142</v>
       </c>
       <c r="O20" t="s" s="26">
-        <v>236</v>
+        <v>220</v>
       </c>
       <c r="P20" s="32">
         <v>23</v>
@@ -4549,7 +4474,7 @@
         <v>132</v>
       </c>
       <c r="U20" t="s" s="26">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="V20" t="s" s="26">
         <v>146</v>
@@ -4563,7 +4488,7 @@
         <v>29</v>
       </c>
       <c r="C21" t="s" s="31">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D21" t="s" s="26">
         <v>120</v>
@@ -4578,28 +4503,28 @@
         <v>123</v>
       </c>
       <c r="H21" t="s" s="31">
-        <v>237</v>
+        <v>124</v>
       </c>
       <c r="I21" t="s" s="26">
         <v>125</v>
       </c>
       <c r="J21" t="s" s="26">
-        <v>238</v>
+        <v>221</v>
       </c>
       <c r="K21" t="s" s="26">
-        <v>239</v>
+        <v>222</v>
       </c>
       <c r="L21" t="s" s="26">
         <v>128</v>
       </c>
       <c r="M21" t="s" s="26">
-        <v>240</v>
+        <v>223</v>
       </c>
       <c r="N21" t="s" s="26">
         <v>130</v>
       </c>
       <c r="O21" t="s" s="26">
-        <v>241</v>
+        <v>224</v>
       </c>
       <c r="P21" s="32">
         <v>22</v>
@@ -4611,13 +4536,13 @@
         <v>29</v>
       </c>
       <c r="S21" t="s" s="26">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="T21" t="s" s="26">
         <v>132</v>
       </c>
       <c r="U21" t="s" s="26">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="V21" t="s" s="26">
         <v>48</v>
@@ -4631,7 +4556,7 @@
         <v>29</v>
       </c>
       <c r="C22" t="s" s="26">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D22" t="s" s="26">
         <v>120</v>
@@ -4646,28 +4571,28 @@
         <v>123</v>
       </c>
       <c r="H22" t="s" s="31">
-        <v>242</v>
+        <v>137</v>
       </c>
       <c r="I22" t="s" s="26">
         <v>138</v>
       </c>
       <c r="J22" t="s" s="26">
-        <v>243</v>
+        <v>225</v>
       </c>
       <c r="K22" t="s" s="26">
-        <v>244</v>
+        <v>226</v>
       </c>
       <c r="L22" t="s" s="26">
         <v>128</v>
       </c>
       <c r="M22" t="s" s="26">
-        <v>245</v>
+        <v>227</v>
       </c>
       <c r="N22" t="s" s="26">
         <v>142</v>
       </c>
       <c r="O22" t="s" s="26">
-        <v>246</v>
+        <v>228</v>
       </c>
       <c r="P22" s="32">
         <v>21</v>
@@ -4679,7 +4604,7 @@
         <v>29</v>
       </c>
       <c r="S22" t="s" s="26">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="T22" t="s" s="26">
         <v>132</v>
@@ -4688,7 +4613,7 @@
         <v>48</v>
       </c>
       <c r="V22" t="s" s="26">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="23" ht="24.65" customHeight="1">
@@ -4714,28 +4639,28 @@
         <v>123</v>
       </c>
       <c r="H23" t="s" s="31">
-        <v>247</v>
+        <v>124</v>
       </c>
       <c r="I23" t="s" s="26">
         <v>125</v>
       </c>
       <c r="J23" t="s" s="26">
-        <v>248</v>
+        <v>229</v>
       </c>
       <c r="K23" t="s" s="26">
-        <v>249</v>
+        <v>230</v>
       </c>
       <c r="L23" t="s" s="26">
         <v>128</v>
       </c>
       <c r="M23" t="s" s="26">
-        <v>250</v>
+        <v>231</v>
       </c>
       <c r="N23" t="s" s="26">
         <v>130</v>
       </c>
       <c r="O23" t="s" s="26">
-        <v>251</v>
+        <v>232</v>
       </c>
       <c r="P23" s="32">
         <v>20</v>
@@ -4753,7 +4678,7 @@
         <v>132</v>
       </c>
       <c r="U23" t="s" s="26">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="V23" t="s" s="26">
         <v>134</v>
@@ -4782,28 +4707,28 @@
         <v>123</v>
       </c>
       <c r="H24" t="s" s="31">
-        <v>252</v>
+        <v>137</v>
       </c>
       <c r="I24" t="s" s="26">
         <v>138</v>
       </c>
       <c r="J24" t="s" s="26">
-        <v>253</v>
+        <v>233</v>
       </c>
       <c r="K24" t="s" s="26">
-        <v>254</v>
+        <v>234</v>
       </c>
       <c r="L24" t="s" s="26">
         <v>128</v>
       </c>
       <c r="M24" t="s" s="26">
-        <v>255</v>
+        <v>235</v>
       </c>
       <c r="N24" t="s" s="26">
         <v>142</v>
       </c>
       <c r="O24" t="s" s="26">
-        <v>256</v>
+        <v>236</v>
       </c>
       <c r="P24" s="32">
         <v>19</v>
@@ -4850,28 +4775,28 @@
         <v>123</v>
       </c>
       <c r="H25" t="s" s="31">
-        <v>257</v>
+        <v>124</v>
       </c>
       <c r="I25" t="s" s="26">
         <v>125</v>
       </c>
       <c r="J25" t="s" s="26">
-        <v>258</v>
+        <v>237</v>
       </c>
       <c r="K25" t="s" s="26">
-        <v>259</v>
+        <v>238</v>
       </c>
       <c r="L25" t="s" s="26">
         <v>128</v>
       </c>
       <c r="M25" t="s" s="26">
-        <v>260</v>
+        <v>239</v>
       </c>
       <c r="N25" t="s" s="26">
         <v>130</v>
       </c>
       <c r="O25" t="s" s="26">
-        <v>261</v>
+        <v>240</v>
       </c>
       <c r="P25" s="32">
         <v>18</v>
@@ -4903,7 +4828,7 @@
         <v>29</v>
       </c>
       <c r="C26" t="s" s="31">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D26" t="s" s="26">
         <v>120</v>
@@ -4918,28 +4843,28 @@
         <v>123</v>
       </c>
       <c r="H26" t="s" s="31">
-        <v>262</v>
+        <v>137</v>
       </c>
       <c r="I26" t="s" s="26">
         <v>138</v>
       </c>
       <c r="J26" t="s" s="26">
-        <v>263</v>
+        <v>241</v>
       </c>
       <c r="K26" t="s" s="26">
-        <v>264</v>
+        <v>242</v>
       </c>
       <c r="L26" t="s" s="26">
         <v>128</v>
       </c>
       <c r="M26" t="s" s="26">
-        <v>265</v>
+        <v>243</v>
       </c>
       <c r="N26" t="s" s="26">
         <v>142</v>
       </c>
       <c r="O26" t="s" s="26">
-        <v>266</v>
+        <v>244</v>
       </c>
       <c r="P26" s="32">
         <v>17</v>
@@ -4957,10 +4882,10 @@
         <v>132</v>
       </c>
       <c r="U26" t="s" s="26">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="V26" t="s" s="26">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="27" ht="24.65" customHeight="1">
@@ -4971,7 +4896,7 @@
         <v>29</v>
       </c>
       <c r="C27" t="s" s="26">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D27" t="s" s="26">
         <v>120</v>
@@ -4986,28 +4911,28 @@
         <v>123</v>
       </c>
       <c r="H27" t="s" s="31">
-        <v>267</v>
+        <v>124</v>
       </c>
       <c r="I27" t="s" s="26">
         <v>125</v>
       </c>
       <c r="J27" t="s" s="26">
-        <v>268</v>
+        <v>245</v>
       </c>
       <c r="K27" t="s" s="26">
-        <v>269</v>
+        <v>246</v>
       </c>
       <c r="L27" t="s" s="26">
         <v>128</v>
       </c>
       <c r="M27" t="s" s="26">
-        <v>270</v>
+        <v>247</v>
       </c>
       <c r="N27" t="s" s="26">
         <v>130</v>
       </c>
       <c r="O27" t="s" s="26">
-        <v>271</v>
+        <v>248</v>
       </c>
       <c r="P27" s="32">
         <v>16</v>
@@ -5019,13 +4944,13 @@
         <v>29</v>
       </c>
       <c r="S27" t="s" s="26">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="T27" t="s" s="26">
         <v>132</v>
       </c>
       <c r="U27" t="s" s="26">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="V27" t="s" s="26">
         <v>134</v>
@@ -5054,28 +4979,28 @@
         <v>123</v>
       </c>
       <c r="H28" t="s" s="31">
-        <v>272</v>
+        <v>137</v>
       </c>
       <c r="I28" t="s" s="26">
         <v>138</v>
       </c>
       <c r="J28" t="s" s="26">
-        <v>273</v>
+        <v>249</v>
       </c>
       <c r="K28" t="s" s="26">
-        <v>274</v>
+        <v>250</v>
       </c>
       <c r="L28" t="s" s="26">
         <v>128</v>
       </c>
       <c r="M28" t="s" s="26">
-        <v>275</v>
+        <v>251</v>
       </c>
       <c r="N28" t="s" s="26">
         <v>142</v>
       </c>
       <c r="O28" t="s" s="26">
-        <v>276</v>
+        <v>252</v>
       </c>
       <c r="P28" s="32">
         <v>15</v>
@@ -5093,7 +5018,7 @@
         <v>132</v>
       </c>
       <c r="U28" t="s" s="26">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="V28" t="s" s="26">
         <v>146</v>
@@ -5122,28 +5047,28 @@
         <v>123</v>
       </c>
       <c r="H29" t="s" s="31">
-        <v>277</v>
+        <v>124</v>
       </c>
       <c r="I29" t="s" s="26">
         <v>125</v>
       </c>
       <c r="J29" t="s" s="26">
-        <v>278</v>
+        <v>253</v>
       </c>
       <c r="K29" t="s" s="26">
-        <v>279</v>
+        <v>254</v>
       </c>
       <c r="L29" t="s" s="26">
         <v>128</v>
       </c>
       <c r="M29" t="s" s="26">
-        <v>280</v>
+        <v>255</v>
       </c>
       <c r="N29" t="s" s="26">
         <v>130</v>
       </c>
       <c r="O29" t="s" s="26">
-        <v>281</v>
+        <v>256</v>
       </c>
       <c r="P29" s="32">
         <v>14</v>

</xml_diff>